<commit_message>
case : update sidebar(admin+sales)+crud cluster shop
</commit_message>
<xml_diff>
--- a/uploads/excelcompany.xlsx
+++ b/uploads/excelcompany.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\first\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E091C98-50FF-4EF6-AEB5-333210FDF924}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441736F2-6C9E-4731-9262-99A3B467294B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID_Company</t>
   </si>
@@ -69,9 +69,6 @@
     <t>firststep11@gmail.com</t>
   </si>
   <si>
-    <t>รัฐวิสาหกิจ</t>
-  </si>
-  <si>
     <t>คุณณัฐวัฒน์</t>
   </si>
   <si>
@@ -84,16 +81,16 @@
     <t>ค้างจ่ายอยู่ 2 อินวอยน์</t>
   </si>
   <si>
-    <t>FIRST</t>
-  </si>
-  <si>
     <t>ภาคเอกชน</t>
   </si>
   <si>
     <t>ไม่ใช่</t>
   </si>
   <si>
-    <t>ใช่</t>
+    <t>PROVINCE_ID</t>
+  </si>
+  <si>
+    <t>AMPHUR_ID</t>
   </si>
 </sst>
 </file>
@@ -479,30 +476,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="2"/>
     <col min="2" max="2" width="13.8984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1"/>
-    <col min="5" max="5" width="17.09765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.09765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.8984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.3984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="2"/>
-    <col min="10" max="10" width="22.59765625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="10.69921875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="17.09765625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="12" style="2"/>
+    <col min="3" max="5" width="18.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1"/>
+    <col min="7" max="7" width="17.09765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.09765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.8984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.3984375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="2"/>
+    <col min="12" max="12" width="22.59765625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.69921875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="17.09765625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="12" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -513,178 +510,165 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>222</v>
+        <v>4254</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
         <v>1234567890</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5">
+      <c r="H2" s="5">
         <v>1234567891233</v>
       </c>
-      <c r="G2" s="6">
+      <c r="I2" s="6">
         <v>15000</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>223</v>
-      </c>
-      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1234567890</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1234567891233</v>
-      </c>
-      <c r="G3" s="6">
-        <v>15000</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{7457CDA7-F2F6-4858-A68B-6FCB86AFE8A5}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{D76811FC-55AD-4053-B7EA-D97D281DFC35}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{7457CDA7-F2F6-4858-A68B-6FCB86AFE8A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>